<commit_message>
adding company life cycle chapter
</commit_message>
<xml_diff>
--- a/BalanceSheet.xlsx
+++ b/BalanceSheet.xlsx
@@ -4,11 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="53">
   <si>
     <t>Revenue</t>
   </si>
@@ -125,6 +127,60 @@
   </si>
   <si>
     <t>EQUITY (10K)</t>
+  </si>
+  <si>
+    <t>8K</t>
+  </si>
+  <si>
+    <t>12K</t>
+  </si>
+  <si>
+    <t>Depreciation and Amortization</t>
+  </si>
+  <si>
+    <t>25K</t>
+  </si>
+  <si>
+    <t>3K</t>
+  </si>
+  <si>
+    <t>1K</t>
+  </si>
+  <si>
+    <t>EBIT = 28K</t>
+  </si>
+  <si>
+    <t>EBITDA = 33K</t>
+  </si>
+  <si>
+    <t>Income statement</t>
+  </si>
+  <si>
+    <t>IDEA</t>
+  </si>
+  <si>
+    <t>Unique Strength</t>
+  </si>
+  <si>
+    <t>Asset</t>
+  </si>
+  <si>
+    <t>Equity</t>
+  </si>
+  <si>
+    <t>200K shares</t>
+  </si>
+  <si>
+    <t>Pre Money</t>
+  </si>
+  <si>
+    <t>500M</t>
+  </si>
+  <si>
+    <t>1M shares</t>
+  </si>
+  <si>
+    <t>Post Money</t>
   </si>
 </sst>
 </file>
@@ -148,7 +204,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -209,8 +265,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="20">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -473,11 +553,168 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -520,6 +757,41 @@
     <xf numFmtId="3" fontId="0" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="1" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="6" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="6" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -549,15 +821,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -565,8 +828,78 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -865,10 +1198,10 @@
   </cols>
   <sheetData>
     <row r="5" spans="8:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H5" s="33" t="s">
+      <c r="H5" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="33"/>
+      <c r="I5" s="48"/>
     </row>
     <row r="6" spans="8:12" x14ac:dyDescent="0.25">
       <c r="H6" s="1" t="s">
@@ -893,10 +1226,10 @@
       <c r="I8" s="10">
         <v>2000000</v>
       </c>
-      <c r="K8" s="24" t="s">
+      <c r="K8" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="L8" s="27" t="s">
+      <c r="L8" s="42" t="s">
         <v>11</v>
       </c>
     </row>
@@ -907,8 +1240,8 @@
       <c r="I9" s="6">
         <v>-500000</v>
       </c>
-      <c r="K9" s="25"/>
-      <c r="L9" s="28"/>
+      <c r="K9" s="40"/>
+      <c r="L9" s="43"/>
     </row>
     <row r="10" spans="8:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H10" s="7" t="s">
@@ -917,8 +1250,8 @@
       <c r="I10" s="8">
         <v>-200000</v>
       </c>
-      <c r="K10" s="25"/>
-      <c r="L10" s="29"/>
+      <c r="K10" s="40"/>
+      <c r="L10" s="44"/>
     </row>
     <row r="11" spans="8:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H11" s="3" t="s">
@@ -927,8 +1260,8 @@
       <c r="I11" s="4">
         <v>-300000</v>
       </c>
-      <c r="K11" s="25"/>
-      <c r="L11" s="30" t="s">
+      <c r="K11" s="40"/>
+      <c r="L11" s="45" t="s">
         <v>12</v>
       </c>
     </row>
@@ -939,8 +1272,8 @@
       <c r="I12" s="10">
         <v>1000000</v>
       </c>
-      <c r="K12" s="25"/>
-      <c r="L12" s="31"/>
+      <c r="K12" s="40"/>
+      <c r="L12" s="46"/>
     </row>
     <row r="13" spans="8:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H13" s="5" t="s">
@@ -949,8 +1282,8 @@
       <c r="I13" s="6">
         <v>-500000</v>
       </c>
-      <c r="K13" s="26"/>
-      <c r="L13" s="32"/>
+      <c r="K13" s="41"/>
+      <c r="L13" s="47"/>
     </row>
     <row r="14" spans="8:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H14" s="3" t="s">
@@ -984,8 +1317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1017,14 +1350,14 @@
       <c r="D4" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="37" t="s">
+      <c r="F4" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="38"/>
-      <c r="I4" s="37" t="s">
+      <c r="G4" s="50"/>
+      <c r="I4" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="J4" s="38"/>
+      <c r="J4" s="50"/>
     </row>
     <row r="5" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
@@ -1047,16 +1380,16 @@
       <c r="D6" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="24" t="s">
+      <c r="F6" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="30" t="s">
+      <c r="G6" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="I6" s="39" t="s">
+      <c r="I6" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="J6" s="34" t="s">
+      <c r="J6" s="51" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1070,12 +1403,12 @@
       <c r="D7" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="25"/>
-      <c r="G7" s="31"/>
-      <c r="I7" s="24" t="s">
+      <c r="F7" s="40"/>
+      <c r="G7" s="46"/>
+      <c r="I7" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="J7" s="35"/>
+      <c r="J7" s="52"/>
     </row>
     <row r="8" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="20" t="s">
@@ -1087,10 +1420,10 @@
       <c r="D8" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="25"/>
-      <c r="G8" s="31"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="35"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="46"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="52"/>
     </row>
     <row r="9" spans="2:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="9" t="s">
@@ -1102,10 +1435,10 @@
       <c r="D9" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="25"/>
-      <c r="G9" s="31"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="35"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="46"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="52"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
@@ -1117,10 +1450,10 @@
       <c r="D10" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="25"/>
-      <c r="G10" s="31"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="35"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="46"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="52"/>
     </row>
     <row r="11" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="22" t="s">
@@ -1132,10 +1465,10 @@
       <c r="D11" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="F11" s="26"/>
-      <c r="G11" s="32"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="36"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="47"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="53"/>
     </row>
     <row r="12" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
@@ -1147,8 +1480,8 @@
       <c r="D12" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="I12" s="26"/>
-      <c r="J12" s="40" t="s">
+      <c r="I12" s="41"/>
+      <c r="J12" s="25" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1174,4 +1507,278 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:E15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="38" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="34"/>
+      <c r="B8" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="35"/>
+    </row>
+    <row r="9" spans="1:5" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="54" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="55"/>
+      <c r="E10" s="57" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="56"/>
+      <c r="E11" s="58"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="E10:E11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C4:G16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="15.5703125" style="60" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" style="60" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="59" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" style="59" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F4" s="60" t="s">
+        <v>46</v>
+      </c>
+      <c r="G4" s="60" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="F5" s="69" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" s="72" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="F6" s="70"/>
+      <c r="G6" s="73"/>
+    </row>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="F7" s="70"/>
+      <c r="G7" s="73"/>
+    </row>
+    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="F8" s="70"/>
+      <c r="G8" s="73"/>
+    </row>
+    <row r="9" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="60" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="60" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="71"/>
+      <c r="G9" s="74"/>
+    </row>
+    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C10" s="61" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="65" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="61" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" s="65" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C11" s="62"/>
+      <c r="D11" s="66" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="62"/>
+      <c r="G11" s="66" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C12" s="62"/>
+      <c r="D12" s="66" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" s="62"/>
+      <c r="G12" s="66" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="63"/>
+      <c r="D13" s="66" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" s="63"/>
+      <c r="G13" s="66" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="3:7" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="64" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="67" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="64" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" s="67" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C16" s="68" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="68"/>
+      <c r="F16" s="68" t="s">
+        <v>52</v>
+      </c>
+      <c r="G16" s="68"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="F10:F13"/>
+    <mergeCell ref="F5:F9"/>
+    <mergeCell ref="G5:G9"/>
+    <mergeCell ref="F16:G16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>